<commit_message>
cambios en model usercategory
</commit_message>
<xml_diff>
--- a/data/documentos/actividades.xlsx
+++ b/data/documentos/actividades.xlsx
@@ -239,16 +239,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,24 +548,24 @@
         <v>42</v>
       </c>
       <c r="B1" s="5"/>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="4"/>
       <c r="C2" s="2" t="s">
         <v>37</v>
       </c>
@@ -576,8 +576,8 @@
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
@@ -586,8 +586,8 @@
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
@@ -598,8 +598,8 @@
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
@@ -610,8 +610,8 @@
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
@@ -622,8 +622,8 @@
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
@@ -634,8 +634,8 @@
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
       <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
@@ -650,16 +650,16 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
@@ -668,8 +668,8 @@
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
       <c r="C11" s="2" t="s">
         <v>6</v>
       </c>
@@ -680,8 +680,8 @@
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
       <c r="C12" s="2" t="s">
         <v>7</v>
       </c>
@@ -690,8 +690,8 @@
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
       <c r="C13" s="2" t="s">
         <v>8</v>
       </c>
@@ -702,10 +702,10 @@
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="6"/>
       <c r="C14" s="1" t="s">
         <v>9</v>
       </c>
@@ -714,8 +714,8 @@
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
       <c r="C15" s="1" t="s">
         <v>10</v>
       </c>
@@ -730,8 +730,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
       <c r="C16" s="1" t="s">
         <v>25</v>
       </c>
@@ -742,8 +742,8 @@
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
       <c r="C17" s="1" t="s">
         <v>11</v>
       </c>
@@ -752,8 +752,8 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
@@ -764,8 +764,8 @@
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
       <c r="C19" s="1" t="s">
         <v>34</v>
       </c>
@@ -776,8 +776,8 @@
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
       <c r="C20" s="1" t="s">
         <v>13</v>
       </c>
@@ -786,8 +786,8 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="1" t="s">
         <v>14</v>
       </c>
@@ -798,8 +798,8 @@
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
       <c r="C22" s="1" t="s">
         <v>31</v>
       </c>
@@ -808,8 +808,8 @@
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
       <c r="C23" s="1" t="s">
         <v>32</v>
       </c>
@@ -820,8 +820,8 @@
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>

</xml_diff>

<commit_message>
cambios para ver categoria, puntos y niveles por usuario
</commit_message>
<xml_diff>
--- a/data/documentos/actividades.xlsx
+++ b/data/documentos/actividades.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t xml:space="preserve"> usertasks -&gt;erick</t>
   </si>
@@ -159,6 +159,15 @@
   </si>
   <si>
     <t>cuantos puntos son por tarea</t>
+  </si>
+  <si>
+    <t>catalogo de logros</t>
+  </si>
+  <si>
+    <t>add,edit.delete achivement</t>
+  </si>
+  <si>
+    <t>getCategoryNextByUser</t>
   </si>
 </sst>
 </file>
@@ -182,7 +191,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,6 +213,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -235,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -249,6 +264,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,7 +736,7 @@
       <c r="C15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -757,7 +774,7 @@
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E18" s="1"/>
@@ -822,10 +839,19 @@
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+      <c r="C24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D26" s="8" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
agrego catalogo de niveles, y metodos en play service
</commit_message>
<xml_diff>
--- a/data/documentos/actividades.xlsx
+++ b/data/documentos/actividades.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\gamification\data\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97575F2D-69BC-4970-8500-636F85AB1F88}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t xml:space="preserve"> usertasks -&gt;erick</t>
   </si>
@@ -116,15 +117,9 @@
     <t>cuantos puntos tiene la categoria</t>
   </si>
   <si>
-    <t>getPointsByAchievment</t>
-  </si>
-  <si>
     <t>achivement-&gt;carlos</t>
   </si>
   <si>
-    <t>1.- cuantos puntos tiene una categoria</t>
-  </si>
-  <si>
     <t>getAchievmentsByCategory</t>
   </si>
   <si>
@@ -164,16 +159,28 @@
     <t>catalogo de logros</t>
   </si>
   <si>
-    <t>add,edit.delete achivement</t>
-  </si>
-  <si>
     <t>getCategoryNextByUser</t>
+  </si>
+  <si>
+    <t>addachivement</t>
+  </si>
+  <si>
+    <t>editachivement</t>
+  </si>
+  <si>
+    <t>deleteachivement</t>
+  </si>
+  <si>
+    <t>1.- cuantos puntos tiene un logro</t>
+  </si>
+  <si>
+    <t>getAllCategory</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -223,7 +230,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -246,26 +253,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,56 +564,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="62.5703125" customWidth="1"/>
-    <col min="4" max="4" width="31.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.42578125" customWidth="1"/>
+    <col min="3" max="3" width="62.54296875" customWidth="1"/>
+    <col min="4" max="4" width="31.54296875" customWidth="1"/>
+    <col min="5" max="5" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="5"/>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="7"/>
       <c r="C1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="4"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="6"/>
       <c r="C2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
@@ -602,9 +621,9 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
@@ -614,9 +633,9 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
@@ -626,9 +645,9 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
@@ -638,9 +657,9 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
@@ -650,9 +669,9 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
@@ -663,20 +682,20 @@
         <v>27</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
@@ -684,9 +703,9 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
       <c r="C11" s="2" t="s">
         <v>6</v>
       </c>
@@ -696,9 +715,9 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
       <c r="C12" s="2" t="s">
         <v>7</v>
       </c>
@@ -706,9 +725,9 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
       <c r="C13" s="2" t="s">
         <v>8</v>
       </c>
@@ -718,11 +737,11 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="6"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="8"/>
       <c r="C14" s="1" t="s">
         <v>9</v>
       </c>
@@ -730,25 +749,25 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="4" t="s">
         <v>28</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="1" t="s">
         <v>25</v>
       </c>
@@ -758,9 +777,9 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
       <c r="C17" s="1" t="s">
         <v>11</v>
       </c>
@@ -768,33 +787,33 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
       <c r="C19" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
       <c r="C20" s="1" t="s">
         <v>13</v>
       </c>
@@ -802,62 +821,82 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
       <c r="C21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>33</v>
+      <c r="D21" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
       <c r="C22" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
       <c r="C23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>30</v>
+        <v>48</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
       <c r="C24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D26" s="8" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="4" t="s">
         <v>47</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D28" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:B13"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A14:B24"/>
+    <mergeCell ref="A14:B26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>